<commit_message>
updated the glosary and working on graphs
</commit_message>
<xml_diff>
--- a/Events glossary.xlsx
+++ b/Events glossary.xlsx
@@ -24,13 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Trial start</t>
-  </si>
-  <si>
-    <t>Water</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Miss</t>
   </si>
@@ -62,7 +56,28 @@
     <t>False alarm</t>
   </si>
   <si>
-    <t>Timeout</t>
+    <t>Water no lick</t>
+  </si>
+  <si>
+    <t>Trial start free water</t>
+  </si>
+  <si>
+    <t>Trial aluminum start</t>
+  </si>
+  <si>
+    <t>Trial no Object start</t>
+  </si>
+  <si>
+    <t>Trial: Reward for lick</t>
+  </si>
+  <si>
+    <t>Trial: CR for no lick</t>
+  </si>
+  <si>
+    <t>Trial: No reward</t>
+  </si>
+  <si>
+    <t>Trial: Reward always</t>
   </si>
 </sst>
 </file>
@@ -380,119 +395,167 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>10</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>110</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>66</v>
+        <v>112</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>44</v>
+        <v>130</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>600</v>
+        <v>132</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>400</v>
+        <v>131</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>300</v>
+        <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>555</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>600</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>400</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correct three digits codes
</commit_message>
<xml_diff>
--- a/Events glossary.xlsx
+++ b/Events glossary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Miss</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Trial: Reward always</t>
+  </si>
+  <si>
+    <t>no water</t>
   </si>
 </sst>
 </file>
@@ -395,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,89 +475,97 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>600</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>10</v>
+        <v>400</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>3</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
implemented and tested both white noise and catch trials
</commit_message>
<xml_diff>
--- a/Events glossary.xlsx
+++ b/Events glossary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Miss</t>
   </si>
@@ -50,12 +50,6 @@
     <t>at non position</t>
   </si>
   <si>
-    <t>correct rejection</t>
-  </si>
-  <si>
-    <t>False alarm</t>
-  </si>
-  <si>
     <t>Water no lick</t>
   </si>
   <si>
@@ -81,6 +75,30 @@
   </si>
   <si>
     <t>no water</t>
+  </si>
+  <si>
+    <t>Catch trial</t>
+  </si>
+  <si>
+    <t>white noise</t>
+  </si>
+  <si>
+    <t>no white noise</t>
+  </si>
+  <si>
+    <t>Trial: Attenuated</t>
+  </si>
+  <si>
+    <t>correct rejection attenuated</t>
+  </si>
+  <si>
+    <t>False alarm attenuated</t>
+  </si>
+  <si>
+    <t>correct rejection (no object)</t>
+  </si>
+  <si>
+    <t>False alarm (no object)</t>
   </si>
 </sst>
 </file>
@@ -398,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,7 +432,7 @@
         <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -422,7 +440,7 @@
         <v>102</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -430,7 +448,7 @@
         <v>110</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -438,7 +456,7 @@
         <v>111</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -446,127 +464,175 @@
         <v>112</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>50</v>
+        <v>131</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>600</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>10</v>
+        <v>400</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>3</v>
       </c>
-      <c r="B20" t="s">
-        <v>9</v>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>555</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>444</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>400</v>
+      </c>
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>